<commit_message>
producto 6 version preliminar
</commit_message>
<xml_diff>
--- a/55_Entregable tabulados/intermedios/02_judicatura_fiscalia_tablas.xlsx
+++ b/55_Entregable tabulados/intermedios/02_judicatura_fiscalia_tablas.xlsx
@@ -11,6 +11,7 @@
     <sheet name="tabla02f" sheetId="2" r:id="rId2"/>
     <sheet name="tabla01j" sheetId="3" r:id="rId3"/>
     <sheet name="tabla02j" sheetId="4" r:id="rId4"/>
+    <sheet name="tabla03j" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -1621,4 +1622,181 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>anio</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ingresado</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>resuelto</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>prop_resuelto</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ejecutado</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>prop_ejecutado</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>34</v>
+      </c>
+      <c r="C2">
+        <v>33</v>
+      </c>
+      <c r="D2">
+        <v>97.09999999999999</v>
+      </c>
+      <c r="E2">
+        <v>18</v>
+      </c>
+      <c r="F2">
+        <v>52.9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>52.6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>31</v>
+      </c>
+      <c r="C4">
+        <v>29</v>
+      </c>
+      <c r="D4">
+        <v>93.5</v>
+      </c>
+      <c r="E4">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>38.7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>44</v>
+      </c>
+      <c r="C5">
+        <v>41</v>
+      </c>
+      <c r="D5">
+        <v>93.2</v>
+      </c>
+      <c r="E5">
+        <v>31</v>
+      </c>
+      <c r="F5">
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>67</v>
+      </c>
+      <c r="C6">
+        <v>56</v>
+      </c>
+      <c r="D6">
+        <v>83.59999999999999</v>
+      </c>
+      <c r="E6">
+        <v>31</v>
+      </c>
+      <c r="F6">
+        <v>46.3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>49</v>
+      </c>
+      <c r="C7">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>36.7</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>12.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>